<commit_message>
feat: add weasyprint, zip library to handle convert html to pdf and save
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -76,6 +76,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -135,8 +136,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -266,78 +271,78 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>